<commit_message>
pequenas atualizações no tempo da abertura da conversa
</commit_message>
<xml_diff>
--- a/number_cel.xlsx
+++ b/number_cel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suporte\Documents\p\bot_whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863784AA-3388-41B9-B562-367AB00511D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC96567B-F9AD-43BF-B6A2-76D3F3EBF322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11535" yWindow="960" windowWidth="21600" windowHeight="11295" xr2:uid="{E5EA4D06-32F8-4BB3-A0B1-9AA81912B7C8}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{E5EA4D06-32F8-4BB3-A0B1-9AA81912B7C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>nome</t>
   </si>
@@ -33,10 +33,16 @@
     <t>telefone</t>
   </si>
   <si>
-    <t>Anderson Levi</t>
+    <t>Levi Shiva</t>
   </si>
   <si>
-    <t>Levi Shiva</t>
+    <t>Aldr</t>
+  </si>
+  <si>
+    <t>Vini Mc</t>
+  </si>
+  <si>
+    <t>_gazelinha</t>
   </si>
 </sst>
 </file>
@@ -46,7 +52,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,11 +68,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Google Sans Text"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -78,6 +79,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,16 +111,25 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -429,19 +446,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06933DAA-9C7F-4A02-8FC4-35B759902F50}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,27 +466,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="32.25" customHeight="1">
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>5541987979867</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5571993876055</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5571987229274</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="B4" s="2"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5547992238348</v>
+      </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>5571997042108</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>